<commit_message>
rename headers and updated fields
- renamed headers to match mdlib2ddh
- mapped license to values instead of terms_of_use
</commit_message>
<xml_diff>
--- a/data-raw/ddh_finance_map.xlsx
+++ b/data-raw/ddh_finance_map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>finance_json_key</t>
   </si>
@@ -63,9 +63,6 @@
     <t>field_wbddh_dsttl_upi</t>
   </si>
   <si>
-    <t>field_wbddh_terms_of_use</t>
-  </si>
-  <si>
     <t>Periodicity</t>
   </si>
   <si>
@@ -181,6 +178,12 @@
   </si>
   <si>
     <t>machine_name</t>
+  </si>
+  <si>
+    <t>field_license_wbddh</t>
+  </si>
+  <si>
+    <t>License</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +586,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
@@ -637,197 +640,199 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify lookup column names
</commit_message>
<xml_diff>
--- a/data-raw/ddh_finance_map.xlsx
+++ b/data-raw/ddh_finance_map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb524812\Documents\harvest\fin2ddh-master\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb523589\Programs\fin2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,166 +24,157 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>finance_json_key</t>
   </si>
   <si>
-    <t xml:space="preserve">field_ddh_harvest_src
+    <t>field_ddh_harvest_sys_id</t>
+  </si>
+  <si>
+    <t>field_wbddh_data_type</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>field_wbddh_data_class</t>
+  </si>
+  <si>
+    <t>field_wbddh_dsttl_upi</t>
+  </si>
+  <si>
+    <t>field_freqency</t>
+  </si>
+  <si>
+    <t>field_topic</t>
+  </si>
+  <si>
+    <t>field_granularity_list</t>
+  </si>
+  <si>
+    <t>field_wbddh_country</t>
+  </si>
+  <si>
+    <t>field_wbddh_economy_coverage</t>
+  </si>
+  <si>
+    <t>field_wbddh_languages_supported</t>
+  </si>
+  <si>
+    <t>field_wbddh_collaborator_upi</t>
+  </si>
+  <si>
+    <t>field_wbddh_type_of_license</t>
+  </si>
+  <si>
+    <t>field_wbddh_start_date</t>
+  </si>
+  <si>
+    <t>field_wbddh_end_date</t>
+  </si>
+  <si>
+    <t>field_wbddh_update_frequency</t>
+  </si>
+  <si>
+    <t>field_wbddh_update_schedule</t>
+  </si>
+  <si>
+    <t>field_wbddh_next_expected_update</t>
+  </si>
+  <si>
+    <t>field_ddh_external_contact_email</t>
+  </si>
+  <si>
+    <t>field_wbddh_ds_source</t>
+  </si>
+  <si>
+    <t>field_wbddh_source</t>
+  </si>
+  <si>
+    <t>field_tags</t>
+  </si>
+  <si>
+    <t>field_wbddh_search_tags</t>
+  </si>
+  <si>
+    <t>field_wbddh_citation_text</t>
+  </si>
+  <si>
+    <t>field_wbddh_data_notes</t>
+  </si>
+  <si>
+    <t>field_wbddh_copyright</t>
+  </si>
+  <si>
+    <t>field_wbddh_gps_ccsas</t>
+  </si>
+  <si>
+    <t>field_wbddh_release_date</t>
+  </si>
+  <si>
+    <t>field_wbddh_modified_date</t>
+  </si>
+  <si>
+    <t>field_wbddh_publisher_name</t>
+  </si>
+  <si>
+    <t>field_wbddh_reference_system</t>
+  </si>
+  <si>
+    <t>field_wbddh_time_periods[0].value</t>
+  </si>
+  <si>
+    <t>field_wbddh_time_periods[0].value2</t>
+  </si>
+  <si>
+    <t>machine_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field_ddh_harvest_src_x000D_
 </t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>field_ddh_harvest_sys_id</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>field_wbddh_data_type</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>field_wbddh_data_class</t>
-  </si>
-  <si>
-    <t>field_wbddh_dsttl_upi</t>
-  </si>
-  <si>
-    <t>Periodicity</t>
-  </si>
-  <si>
-    <t>field_freqency</t>
-  </si>
-  <si>
-    <t>field_topic</t>
-  </si>
-  <si>
-    <t>Granularity</t>
-  </si>
-  <si>
-    <t>field_granularity_list</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>field_wbddh_country</t>
-  </si>
-  <si>
-    <t>Economy-Coverage</t>
-  </si>
-  <si>
-    <t>field_wbddh_economy_coverage</t>
-  </si>
-  <si>
-    <t>field_wbddh_languages_supported</t>
-  </si>
-  <si>
-    <t>field_wbddh_collaborator_upi</t>
-  </si>
-  <si>
-    <t>field_wbddh_type_of_license</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>field_wbddh_start_date</t>
-  </si>
-  <si>
-    <t>end_date</t>
-  </si>
-  <si>
-    <t>field_wbddh_end_date</t>
-  </si>
-  <si>
-    <t>Update-Frequency</t>
-  </si>
-  <si>
-    <t>field_wbddh_update_frequency</t>
-  </si>
-  <si>
-    <t>Update-Schedule</t>
-  </si>
-  <si>
-    <t>field_wbddh_update_schedule</t>
-  </si>
-  <si>
-    <t>field_wbddh_next_expected_update</t>
-  </si>
-  <si>
-    <t>field_ddh_external_contact_email</t>
-  </si>
-  <si>
-    <t>field_wbddh_ds_source</t>
-  </si>
-  <si>
-    <t>field_wbddh_source</t>
-  </si>
-  <si>
-    <t>field_tags</t>
-  </si>
-  <si>
-    <t>field_wbddh_search_tags</t>
-  </si>
-  <si>
-    <t>field_wbddh_citation_text</t>
-  </si>
-  <si>
-    <t>field_wbddh_data_notes</t>
-  </si>
-  <si>
-    <t>field_wbddh_copyright</t>
-  </si>
-  <si>
-    <t>field_wbddh_gps_ccsas</t>
-  </si>
-  <si>
-    <t>createdAt</t>
-  </si>
-  <si>
-    <t>field_wbddh_release_date</t>
-  </si>
-  <si>
-    <t>rowsUpdatedAt</t>
-  </si>
-  <si>
-    <t>field_wbddh_modified_date</t>
-  </si>
-  <si>
-    <t>field_wbddh_publisher_name</t>
-  </si>
-  <si>
-    <t>field_wbddh_reference_system</t>
-  </si>
-  <si>
-    <t>field_wbddh_time_periods[0].value</t>
-  </si>
-  <si>
-    <t>field_wbddh_time_periods[0].value2</t>
-  </si>
-  <si>
-    <t>machine_name</t>
-  </si>
-  <si>
-    <t>field_license_wbddh</t>
-  </si>
-  <si>
-    <t>License</t>
+    <t>view/id</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/Additional Information/Type</t>
+  </si>
+  <si>
+    <t>view/name</t>
+  </si>
+  <si>
+    <t>view/description</t>
+  </si>
+  <si>
+    <t>field_wbddh_terms_of_use</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/Additional Information/Periodicity</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/Additional Information/Granularity</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/scope/Country</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/scope/Economy Coverage</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/scope/Update Frequency</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/scope/Update Schedule</t>
+  </si>
+  <si>
+    <t>view/createdAt</t>
+  </si>
+  <si>
+    <t>view/rowsUpdatedAt</t>
   </si>
 </sst>
 </file>
@@ -572,7 +563,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,253 +577,247 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A18" s="6"/>
       <c r="B18" s="7" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A19" s="6"/>
       <c r="B19" s="7" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert to full field names in lookup table
</commit_message>
<xml_diff>
--- a/data-raw/ddh_finance_map.xlsx
+++ b/data-raw/ddh_finance_map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb524812\Documents\harvest\fin2ddh-master\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb523589\Programs\fin2ddh\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,166 +24,157 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>finance_json_key</t>
   </si>
   <si>
-    <t xml:space="preserve">field_ddh_harvest_src
+    <t>field_ddh_harvest_sys_id</t>
+  </si>
+  <si>
+    <t>field_wbddh_data_type</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>field_wbddh_data_class</t>
+  </si>
+  <si>
+    <t>field_wbddh_dsttl_upi</t>
+  </si>
+  <si>
+    <t>field_freqency</t>
+  </si>
+  <si>
+    <t>field_topic</t>
+  </si>
+  <si>
+    <t>field_granularity_list</t>
+  </si>
+  <si>
+    <t>field_wbddh_country</t>
+  </si>
+  <si>
+    <t>field_wbddh_economy_coverage</t>
+  </si>
+  <si>
+    <t>field_wbddh_languages_supported</t>
+  </si>
+  <si>
+    <t>field_wbddh_collaborator_upi</t>
+  </si>
+  <si>
+    <t>field_wbddh_type_of_license</t>
+  </si>
+  <si>
+    <t>field_wbddh_start_date</t>
+  </si>
+  <si>
+    <t>field_wbddh_end_date</t>
+  </si>
+  <si>
+    <t>field_wbddh_update_frequency</t>
+  </si>
+  <si>
+    <t>field_wbddh_update_schedule</t>
+  </si>
+  <si>
+    <t>field_wbddh_next_expected_update</t>
+  </si>
+  <si>
+    <t>field_ddh_external_contact_email</t>
+  </si>
+  <si>
+    <t>field_wbddh_ds_source</t>
+  </si>
+  <si>
+    <t>field_wbddh_source</t>
+  </si>
+  <si>
+    <t>field_tags</t>
+  </si>
+  <si>
+    <t>field_wbddh_search_tags</t>
+  </si>
+  <si>
+    <t>field_wbddh_citation_text</t>
+  </si>
+  <si>
+    <t>field_wbddh_data_notes</t>
+  </si>
+  <si>
+    <t>field_wbddh_copyright</t>
+  </si>
+  <si>
+    <t>field_wbddh_gps_ccsas</t>
+  </si>
+  <si>
+    <t>field_wbddh_release_date</t>
+  </si>
+  <si>
+    <t>field_wbddh_modified_date</t>
+  </si>
+  <si>
+    <t>field_wbddh_publisher_name</t>
+  </si>
+  <si>
+    <t>field_wbddh_reference_system</t>
+  </si>
+  <si>
+    <t>field_wbddh_time_periods[0].value</t>
+  </si>
+  <si>
+    <t>field_wbddh_time_periods[0].value2</t>
+  </si>
+  <si>
+    <t>machine_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field_ddh_harvest_src_x000D_
 </t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>field_ddh_harvest_sys_id</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>field_wbddh_data_type</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>body</t>
-  </si>
-  <si>
-    <t>field_wbddh_data_class</t>
-  </si>
-  <si>
-    <t>field_wbddh_dsttl_upi</t>
-  </si>
-  <si>
-    <t>Periodicity</t>
-  </si>
-  <si>
-    <t>field_freqency</t>
-  </si>
-  <si>
-    <t>field_topic</t>
-  </si>
-  <si>
-    <t>Granularity</t>
-  </si>
-  <si>
-    <t>field_granularity_list</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>field_wbddh_country</t>
-  </si>
-  <si>
-    <t>Economy-Coverage</t>
-  </si>
-  <si>
-    <t>field_wbddh_economy_coverage</t>
-  </si>
-  <si>
-    <t>field_wbddh_languages_supported</t>
-  </si>
-  <si>
-    <t>field_wbddh_collaborator_upi</t>
-  </si>
-  <si>
-    <t>field_wbddh_type_of_license</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>field_wbddh_start_date</t>
-  </si>
-  <si>
-    <t>end_date</t>
-  </si>
-  <si>
-    <t>field_wbddh_end_date</t>
-  </si>
-  <si>
-    <t>Update-Frequency</t>
-  </si>
-  <si>
-    <t>field_wbddh_update_frequency</t>
-  </si>
-  <si>
-    <t>Update-Schedule</t>
-  </si>
-  <si>
-    <t>field_wbddh_update_schedule</t>
-  </si>
-  <si>
-    <t>field_wbddh_next_expected_update</t>
-  </si>
-  <si>
-    <t>field_ddh_external_contact_email</t>
-  </si>
-  <si>
-    <t>field_wbddh_ds_source</t>
-  </si>
-  <si>
-    <t>field_wbddh_source</t>
-  </si>
-  <si>
-    <t>field_tags</t>
-  </si>
-  <si>
-    <t>field_wbddh_search_tags</t>
-  </si>
-  <si>
-    <t>field_wbddh_citation_text</t>
-  </si>
-  <si>
-    <t>field_wbddh_data_notes</t>
-  </si>
-  <si>
-    <t>field_wbddh_copyright</t>
-  </si>
-  <si>
-    <t>field_wbddh_gps_ccsas</t>
-  </si>
-  <si>
-    <t>createdAt</t>
-  </si>
-  <si>
-    <t>field_wbddh_release_date</t>
-  </si>
-  <si>
-    <t>rowsUpdatedAt</t>
-  </si>
-  <si>
-    <t>field_wbddh_modified_date</t>
-  </si>
-  <si>
-    <t>field_wbddh_publisher_name</t>
-  </si>
-  <si>
-    <t>field_wbddh_reference_system</t>
-  </si>
-  <si>
-    <t>field_wbddh_time_periods[0].value</t>
-  </si>
-  <si>
-    <t>field_wbddh_time_periods[0].value2</t>
-  </si>
-  <si>
-    <t>machine_name</t>
-  </si>
-  <si>
-    <t>field_license_wbddh</t>
-  </si>
-  <si>
-    <t>License</t>
+    <t>view/id</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/Additional Information/Type</t>
+  </si>
+  <si>
+    <t>view/name</t>
+  </si>
+  <si>
+    <t>view/description</t>
+  </si>
+  <si>
+    <t>field_wbddh_terms_of_use</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/Additional Information/Periodicity</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/Additional Information/Granularity</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/scope/Country</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/scope/Economy Coverage</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/scope/Update Frequency</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/scope/Update Schedule</t>
+  </si>
+  <si>
+    <t>view/createdAt</t>
+  </si>
+  <si>
+    <t>view/rowsUpdatedAt</t>
   </si>
 </sst>
 </file>
@@ -572,7 +563,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,253 +577,247 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A18" s="6"/>
       <c r="B18" s="7" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A19" s="6"/>
       <c r="B19" s="7" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated frequency to periodicity
</commit_message>
<xml_diff>
--- a/data-raw/ddh_finance_map.xlsx
+++ b/data-raw/ddh_finance_map.xlsx
@@ -174,7 +174,7 @@
     <t>view/rowsUpdatedAt</t>
   </si>
   <si>
-    <t>field_frequency</t>
+    <t>field_wbddh_periodicity</t>
   </si>
 </sst>
 </file>
@@ -198,14 +198,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -234,18 +237,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,144 +568,145 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7" t="s">
+    <row r="18" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -708,7 +714,7 @@
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -716,67 +722,67 @@
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -784,7 +790,7 @@
       <c r="A32" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -792,31 +798,31 @@
       <c r="A33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="9" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update lookup table to "additional information"
</commit_message>
<xml_diff>
--- a/data-raw/ddh_finance_map.xlsx
+++ b/data-raw/ddh_finance_map.xlsx
@@ -155,15 +155,6 @@
     <t>view/metadata/custom_fields/scope/Country</t>
   </si>
   <si>
-    <t>view/metadata/custom_fields/scope/Economy Coverage</t>
-  </si>
-  <si>
-    <t>view/metadata/custom_fields/scope/Update Frequency</t>
-  </si>
-  <si>
-    <t>view/metadata/custom_fields/scope/Update Schedule</t>
-  </si>
-  <si>
     <t>view/createdAt</t>
   </si>
   <si>
@@ -174,6 +165,15 @@
   </si>
   <si>
     <t>field_ddh_harvest_src</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/Additional Information/Economy Coverage</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/Additional Information/Update Frequency</t>
+  </si>
+  <si>
+    <t>view/metadata/custom_fields/Additional Information/Update Schedule</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +588,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>10</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>16</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>17</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>28</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
update periodicity to frequency
</commit_message>
<xml_diff>
--- a/data-raw/ddh_finance_map.xlsx
+++ b/data-raw/ddh_finance_map.xlsx
@@ -161,9 +161,6 @@
     <t>view/rowsUpdatedAt</t>
   </si>
   <si>
-    <t>field_wbddh_periodicity</t>
-  </si>
-  <si>
     <t>field_ddh_harvest_src</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>view/metadata/custom_fields/Additional Information/Update Schedule</t>
+  </si>
+  <si>
+    <t>field_frequency</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +588,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>10</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>16</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>17</v>

</xml_diff>